<commit_message>
Updated scripts and analysis results
</commit_message>
<xml_diff>
--- a/analysis/normalisation/2016-03-09/64norms.xlsx
+++ b/analysis/normalisation/2016-03-09/64norms.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="64norms.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
   <si>
     <t>d</t>
   </si>
@@ -214,14 +215,24 @@
   <si>
     <t>ws</t>
   </si>
+  <si>
+    <t>MAX</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -248,8 +259,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AR108" sqref="AR108"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:XFD102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20115,4 +20135,439 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
+    <col min="2" max="18" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.622</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.62699999999999989</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.55699999999999994</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.49600000000000011</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.66699999999999993</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.46499999999999969</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.54699999999999993</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.71299999999999986</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.503</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.55499999999999983</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.69100000000000006</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.496</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.64699999999999991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>0.6389999999999999</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.68999999999999972</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.505</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.59799999999999986</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.65899999999999981</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.45700000000000007</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.6379999999999999</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.57699999999999985</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.622</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.6339999999999999</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0.62599999999999989</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.57199999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>0.73799999999999988</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.56299999999999983</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.57699999999999985</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.70599999999999985</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.5369999999999997</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.55899999999999994</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.75100000000000011</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.73900000000000021</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.55200000000000016</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.6409999999999999</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.59899999999999987</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.73699999999999977</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0.57700000000000007</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.60999999999999988</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>0.69699999999999984</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.6349999999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.58900000000000008</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.74900000000000011</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.55800000000000016</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.71700000000000019</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>0.75100000000000011</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:R2 A4:R4 A6:R6 A8:I8 A10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>